<commit_message>
Documentos de mapeamento criados
</commit_message>
<xml_diff>
--- a/Documentos/Mapeamento das Fontes de Dados/2CX/MAPEAMENTO_2CX.xlsx
+++ b/Documentos/Mapeamento das Fontes de Dados/2CX/MAPEAMENTO_2CX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\int.matheus\Desktop\DW\Data-Warehouse\Documentos\Mapeamento das Fontes de Dados\2CX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49059761-1FAC-4FDC-8E6A-23C38BD9D421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EE3B35-95AA-4F81-B762-8C4395EE948B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="685" firstSheet="2" activeTab="2" xr2:uid="{40AA39DE-57CF-4226-99BA-0B59FFBB7B19}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="685" firstSheet="2" activeTab="2" xr2:uid="{40AA39DE-57CF-4226-99BA-0B59FFBB7B19}"/>
   </bookViews>
   <sheets>
     <sheet name="PAINEL" sheetId="18" state="hidden" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1901" uniqueCount="467">
   <si>
     <t>CPF</t>
   </si>
@@ -1440,6 +1440,18 @@
   </si>
   <si>
     <t>2CX É APENAS ATIVO</t>
+  </si>
+  <si>
+    <t>queues</t>
+  </si>
+  <si>
+    <t>chamadas.fila cruzando com o queues.fila</t>
+  </si>
+  <si>
+    <t>terminator</t>
+  </si>
+  <si>
+    <t>replica_mfrflab1 , replica_mfrfl2b1, replica_mfrfl3b1</t>
   </si>
 </sst>
 </file>
@@ -1766,7 +1778,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1896,9 +1908,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6712,10 +6721,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62AE222-1740-4697-9DDD-8C113A0027CC}">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="70.77734375" defaultRowHeight="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6968,13 +6977,13 @@
       </c>
       <c r="G7" s="38"/>
       <c r="H7" s="38" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
       <c r="I7" s="38" t="s">
         <v>446</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="K7" s="38"/>
       <c r="L7" s="38"/>
@@ -7006,7 +7015,7 @@
       </c>
       <c r="G8" s="38"/>
       <c r="H8" s="38" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
       <c r="I8" s="38" t="s">
         <v>446</v>
@@ -7044,7 +7053,7 @@
       </c>
       <c r="G9" s="38"/>
       <c r="H9" s="38" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
       <c r="I9" s="38" t="s">
         <v>457</v>
@@ -7084,7 +7093,7 @@
       </c>
       <c r="G10" s="38"/>
       <c r="H10" s="38" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
       <c r="I10" s="38" t="s">
         <v>449</v>
@@ -7122,7 +7131,7 @@
       </c>
       <c r="G11" s="38"/>
       <c r="H11" s="38" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
       <c r="I11" s="38" t="s">
         <v>446</v>
@@ -7160,7 +7169,7 @@
       </c>
       <c r="G12" s="38"/>
       <c r="H12" s="38" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
       <c r="I12" s="38" t="s">
         <v>446</v>
@@ -7180,32 +7189,36 @@
       <c r="R12" s="38"/>
     </row>
     <row r="13" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="38" t="s">
         <v>438</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="38" t="s">
         <v>439</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="38" t="s">
         <v>355</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44">
+      <c r="D13" s="38"/>
+      <c r="E13" s="38">
         <v>200</v>
       </c>
-      <c r="F13" s="44" t="s">
+      <c r="F13" s="38" t="s">
         <v>444</v>
       </c>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44" t="s">
-        <v>445</v>
-      </c>
-      <c r="I13" s="44" t="s">
-        <v>446</v>
-      </c>
-      <c r="J13" s="44"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38" t="s">
+        <v>466</v>
+      </c>
+      <c r="I13" s="38" t="s">
+        <v>463</v>
+      </c>
+      <c r="J13" s="38" t="s">
+        <v>459</v>
+      </c>
       <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
+      <c r="L13" s="38" t="s">
+        <v>464</v>
+      </c>
       <c r="M13" s="38"/>
       <c r="N13" s="38" t="s">
         <v>430</v>
@@ -7234,7 +7247,7 @@
       </c>
       <c r="G14" s="38"/>
       <c r="H14" s="38" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
       <c r="I14" s="38" t="s">
         <v>446</v>
@@ -7272,7 +7285,7 @@
       </c>
       <c r="G15" s="38"/>
       <c r="H15" s="38" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
       <c r="I15" s="38" t="s">
         <v>446</v>
@@ -7310,7 +7323,7 @@
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="38" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
       <c r="I16" s="38" t="s">
         <v>446</v>
@@ -7348,7 +7361,7 @@
       </c>
       <c r="G17" s="38"/>
       <c r="H17" s="38" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
       <c r="I17" s="38" t="s">
         <v>446</v>
@@ -7368,30 +7381,32 @@
       <c r="R17" s="38"/>
     </row>
     <row r="18" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="38" t="s">
         <v>355</v>
       </c>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44">
+      <c r="D18" s="38"/>
+      <c r="E18" s="38">
         <v>20</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="F18" s="38" t="s">
         <v>444</v>
       </c>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44" t="s">
-        <v>445</v>
-      </c>
-      <c r="I18" s="44" t="s">
+      <c r="G18" s="38"/>
+      <c r="H18" s="38" t="s">
+        <v>466</v>
+      </c>
+      <c r="I18" s="38" t="s">
         <v>446</v>
       </c>
-      <c r="J18" s="44"/>
+      <c r="J18" s="38" t="s">
+        <v>465</v>
+      </c>
       <c r="K18" s="38"/>
       <c r="L18" s="38"/>
       <c r="M18" s="38"/>
@@ -7422,7 +7437,7 @@
       </c>
       <c r="G19" s="38"/>
       <c r="H19" s="38" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
       <c r="I19" s="38" t="s">
         <v>446</v>
@@ -7460,7 +7475,7 @@
       </c>
       <c r="G20" s="38"/>
       <c r="H20" s="38" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
       <c r="I20" s="38" t="s">
         <v>446</v>
@@ -7481,37 +7496,29 @@
     </row>
     <row r="21" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="38" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="D21" s="38"/>
       <c r="E21" s="38">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F21" s="38" t="s">
         <v>444</v>
       </c>
       <c r="G21" s="38"/>
-      <c r="H21" s="38" t="s">
-        <v>445</v>
-      </c>
-      <c r="I21" s="38" t="s">
-        <v>446</v>
-      </c>
-      <c r="J21" s="38" t="s">
-        <v>455</v>
-      </c>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
       <c r="K21" s="38"/>
       <c r="L21" s="38"/>
       <c r="M21" s="38"/>
-      <c r="N21" s="38" t="s">
-        <v>430</v>
-      </c>
+      <c r="N21" s="38"/>
       <c r="O21" s="38"/>
       <c r="P21" s="38"/>
       <c r="Q21" s="38"/>
@@ -7519,17 +7526,17 @@
     </row>
     <row r="22" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="38" t="s">
-        <v>185</v>
+        <v>56</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="D22" s="38"/>
       <c r="E22" s="38">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F22" s="38" t="s">
         <v>444</v>
@@ -7538,14 +7545,10 @@
       <c r="H22" s="38"/>
       <c r="I22" s="38"/>
       <c r="J22" s="38"/>
-      <c r="K22" s="38" t="s">
-        <v>462</v>
-      </c>
+      <c r="K22" s="38"/>
       <c r="L22" s="38"/>
       <c r="M22" s="38"/>
-      <c r="N22" s="38" t="s">
-        <v>430</v>
-      </c>
+      <c r="N22" s="38"/>
       <c r="O22" s="38"/>
       <c r="P22" s="38"/>
       <c r="Q22" s="38"/>
@@ -7553,25 +7556,31 @@
     </row>
     <row r="23" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="38" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>180</v>
+        <v>355</v>
       </c>
       <c r="D23" s="38"/>
       <c r="E23" s="38">
-        <v>19.2</v>
+        <v>11</v>
       </c>
       <c r="F23" s="38" t="s">
         <v>444</v>
       </c>
       <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
+      <c r="H23" s="38" t="s">
+        <v>466</v>
+      </c>
+      <c r="I23" s="38" t="s">
+        <v>446</v>
+      </c>
+      <c r="J23" s="38" t="s">
+        <v>455</v>
+      </c>
       <c r="K23" s="38"/>
       <c r="L23" s="38"/>
       <c r="M23" s="38"/>
@@ -7582,6 +7591,72 @@
       <c r="P23" s="38"/>
       <c r="Q23" s="38"/>
       <c r="R23" s="38"/>
+    </row>
+    <row r="24" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38">
+        <v>11</v>
+      </c>
+      <c r="F24" s="38" t="s">
+        <v>444</v>
+      </c>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38" t="s">
+        <v>462</v>
+      </c>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38" t="s">
+        <v>430</v>
+      </c>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
+    </row>
+    <row r="25" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38">
+        <v>19.2</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>444</v>
+      </c>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38" t="s">
+        <v>430</v>
+      </c>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Mapeamento atualizado com PK
</commit_message>
<xml_diff>
--- a/Documentos/Mapeamento das Fontes de Dados/2CX/MAPEAMENTO_2CX.xlsx
+++ b/Documentos/Mapeamento das Fontes de Dados/2CX/MAPEAMENTO_2CX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\int.matheus\Desktop\DW\Data-Warehouse\Documentos\Mapeamento das Fontes de Dados\2CX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDE9716-D7FF-42AF-87D1-3B1C673D4072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DB35DB-6EF8-44C7-8B83-589CB1B8614A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="685" firstSheet="2" activeTab="2" xr2:uid="{40AA39DE-57CF-4226-99BA-0B59FFBB7B19}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="428">
   <si>
     <t>CPF</t>
   </si>
@@ -1195,9 +1195,6 @@
     <t>QUERY</t>
   </si>
   <si>
-    <t>TIM</t>
-  </si>
-  <si>
     <t>CPF DO CLIENTE</t>
   </si>
   <si>
@@ -1322,6 +1319,18 @@
   </si>
   <si>
     <t>NVARCHAR</t>
+  </si>
+  <si>
+    <t>DATA_INSERT</t>
+  </si>
+  <si>
+    <t>MOMENTO QUE O DADO FOI INSERIDO NA TABELA</t>
+  </si>
+  <si>
+    <t>DATETIMENOW()</t>
+  </si>
+  <si>
+    <t>PK</t>
   </si>
 </sst>
 </file>
@@ -1515,7 +1524,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1628,12 +1637,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1750,6 +1796,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2290,17 +2345,17 @@
       <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="43" t="s">
         <v>362</v>
       </c>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
     </row>
     <row r="5" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
@@ -2730,17 +2785,17 @@
       <c r="O3" s="16"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="J4" s="40" t="s">
+      <c r="J4" s="43" t="s">
         <v>362</v>
       </c>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
@@ -4964,10 +5019,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62AE222-1740-4697-9DDD-8C113A0027CC}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7:L7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="70.77734375" defaultRowHeight="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5052,26 +5107,24 @@
       </c>
       <c r="E2" s="36"/>
       <c r="F2" s="36" t="s">
+        <v>393</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>415</v>
+      </c>
+      <c r="H2" s="36" t="s">
         <v>394</v>
       </c>
-      <c r="G2" s="36" t="s">
-        <v>416</v>
-      </c>
-      <c r="H2" s="36" t="s">
+      <c r="I2" s="36" t="s">
         <v>395</v>
       </c>
-      <c r="I2" s="36" t="s">
-        <v>396</v>
-      </c>
       <c r="J2" s="36" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K2" s="36"/>
       <c r="L2" s="36"/>
       <c r="M2" s="36"/>
-      <c r="N2" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N2" s="36"/>
       <c r="O2" s="36"/>
       <c r="P2" s="36"/>
       <c r="Q2" s="36"/>
@@ -5082,36 +5135,34 @@
         <v>46</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D3" s="36">
         <v>20</v>
       </c>
       <c r="E3" s="36"/>
       <c r="F3" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J3" s="36" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
       <c r="M3" s="36"/>
-      <c r="N3" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N3" s="36"/>
       <c r="O3" s="36"/>
       <c r="P3" s="36"/>
       <c r="Q3" s="36"/>
@@ -5122,36 +5173,34 @@
         <v>0</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D4" s="36">
         <v>20</v>
       </c>
       <c r="E4" s="36"/>
       <c r="F4" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I4" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K4" s="36"/>
       <c r="L4" s="36"/>
       <c r="M4" s="36"/>
-      <c r="N4" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N4" s="36"/>
       <c r="O4" s="36"/>
       <c r="P4" s="36"/>
       <c r="Q4" s="36"/>
@@ -5159,41 +5208,39 @@
     </row>
     <row r="5" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="36" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D5" s="36">
         <v>30</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G5" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I5" s="36" t="s">
+        <v>405</v>
+      </c>
+      <c r="J5" s="36" t="s">
         <v>406</v>
-      </c>
-      <c r="J5" s="36" t="s">
-        <v>407</v>
       </c>
       <c r="K5" s="36"/>
       <c r="L5" s="36" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="M5" s="36"/>
-      <c r="N5" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N5" s="36"/>
       <c r="O5" s="36"/>
       <c r="P5" s="36"/>
       <c r="Q5" s="36"/>
@@ -5201,39 +5248,37 @@
     </row>
     <row r="6" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="36" t="s">
+        <v>384</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>385</v>
       </c>
-      <c r="B6" s="36" t="s">
-        <v>386</v>
-      </c>
       <c r="C6" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D6" s="36">
         <v>100</v>
       </c>
       <c r="E6" s="36"/>
       <c r="F6" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I6" s="36" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K6" s="36"/>
       <c r="L6" s="36"/>
       <c r="M6" s="36"/>
-      <c r="N6" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N6" s="36"/>
       <c r="O6" s="36"/>
       <c r="P6" s="36"/>
       <c r="Q6" s="36"/>
@@ -5244,36 +5289,36 @@
         <v>215</v>
       </c>
       <c r="B7" s="36" t="s">
+        <v>419</v>
+      </c>
+      <c r="C7" s="36" t="s">
         <v>420</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>421</v>
       </c>
       <c r="D7" s="36">
         <v>19</v>
       </c>
-      <c r="E7" s="36"/>
+      <c r="E7" s="36" t="s">
+        <v>427</v>
+      </c>
       <c r="F7" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G7" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H7" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I7" s="36" t="s">
+        <v>395</v>
+      </c>
+      <c r="J7" s="36" t="s">
         <v>396</v>
-      </c>
-      <c r="J7" s="36" t="s">
-        <v>397</v>
       </c>
       <c r="K7" s="36"/>
       <c r="L7" s="36"/>
       <c r="M7" s="36"/>
-      <c r="N7" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N7" s="36"/>
       <c r="O7" s="36"/>
       <c r="P7" s="36"/>
       <c r="Q7" s="36"/>
@@ -5281,39 +5326,37 @@
     </row>
     <row r="8" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
+        <v>386</v>
+      </c>
+      <c r="B8" s="36" t="s">
         <v>387</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>388</v>
-      </c>
       <c r="C8" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D8" s="36">
         <v>19</v>
       </c>
       <c r="E8" s="36"/>
       <c r="F8" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G8" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I8" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
       <c r="M8" s="36"/>
-      <c r="N8" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N8" s="36"/>
       <c r="O8" s="36"/>
       <c r="P8" s="36"/>
       <c r="Q8" s="36"/>
@@ -5321,41 +5364,39 @@
     </row>
     <row r="9" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="36" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D9" s="36">
         <v>200</v>
       </c>
       <c r="E9" s="36"/>
       <c r="F9" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G9" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H9" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I9" s="36" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K9" s="36"/>
       <c r="L9" s="36" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="M9" s="36"/>
-      <c r="N9" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N9" s="36"/>
       <c r="O9" s="36"/>
       <c r="P9" s="36"/>
       <c r="Q9" s="36"/>
@@ -5363,39 +5404,37 @@
     </row>
     <row r="10" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="36" t="s">
+        <v>389</v>
+      </c>
+      <c r="B10" s="36" t="s">
         <v>390</v>
       </c>
-      <c r="B10" s="36" t="s">
-        <v>391</v>
-      </c>
       <c r="C10" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D10" s="36">
         <v>19</v>
       </c>
       <c r="E10" s="36"/>
       <c r="F10" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I10" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J10" s="36" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="K10" s="36"/>
       <c r="L10" s="36"/>
       <c r="M10" s="36"/>
-      <c r="N10" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N10" s="36"/>
       <c r="O10" s="36"/>
       <c r="P10" s="36"/>
       <c r="Q10" s="36"/>
@@ -5403,39 +5442,37 @@
     </row>
     <row r="11" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="B11" s="36" t="s">
         <v>392</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>393</v>
-      </c>
       <c r="C11" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D11" s="36">
         <v>200</v>
       </c>
       <c r="E11" s="36"/>
       <c r="F11" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G11" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H11" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I11" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J11" s="36" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K11" s="36"/>
       <c r="L11" s="36"/>
       <c r="M11" s="36"/>
-      <c r="N11" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N11" s="36"/>
       <c r="O11" s="36"/>
       <c r="P11" s="36"/>
       <c r="Q11" s="36"/>
@@ -5449,33 +5486,31 @@
         <v>217</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D12" s="36">
         <v>250</v>
       </c>
       <c r="E12" s="36"/>
       <c r="F12" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G12" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H12" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I12" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K12" s="36"/>
       <c r="L12" s="36"/>
       <c r="M12" s="36"/>
-      <c r="N12" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N12" s="36"/>
       <c r="O12" s="36"/>
       <c r="P12" s="36"/>
       <c r="Q12" s="36"/>
@@ -5489,33 +5524,31 @@
         <v>218</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D13" s="36">
         <v>50</v>
       </c>
       <c r="E13" s="36"/>
       <c r="F13" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G13" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H13" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I13" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K13" s="36"/>
       <c r="L13" s="36"/>
       <c r="M13" s="36"/>
-      <c r="N13" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N13" s="36"/>
       <c r="O13" s="36"/>
       <c r="P13" s="36"/>
       <c r="Q13" s="36"/>
@@ -5529,33 +5562,31 @@
         <v>219</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D14" s="36">
         <v>19</v>
       </c>
       <c r="E14" s="36"/>
       <c r="F14" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G14" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H14" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I14" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="K14" s="36"/>
       <c r="L14" s="36"/>
       <c r="M14" s="36"/>
-      <c r="N14" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N14" s="36"/>
       <c r="O14" s="36"/>
       <c r="P14" s="36"/>
       <c r="Q14" s="36"/>
@@ -5569,33 +5600,31 @@
         <v>220</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D15" s="36">
         <v>19</v>
       </c>
       <c r="E15" s="36"/>
       <c r="F15" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H15" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I15" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K15" s="36"/>
       <c r="L15" s="36"/>
       <c r="M15" s="36"/>
-      <c r="N15" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="N15" s="36"/>
       <c r="O15" s="36"/>
       <c r="P15" s="36"/>
       <c r="Q15" s="36"/>
@@ -5609,14 +5638,14 @@
         <v>229</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D16" s="36">
         <v>19</v>
       </c>
       <c r="E16" s="36"/>
       <c r="F16" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
@@ -5639,14 +5668,14 @@
         <v>230</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D17" s="36">
         <v>19</v>
       </c>
       <c r="E17" s="36"/>
       <c r="F17" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G17" s="36"/>
       <c r="H17" s="36"/>
@@ -5669,35 +5698,31 @@
         <v>221</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D18" s="36">
         <v>20</v>
       </c>
       <c r="E18" s="36"/>
       <c r="F18" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G18" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H18" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I18" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J18" s="36" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="K18" s="36"/>
       <c r="L18" s="36"/>
-      <c r="M18" s="38">
-        <v>171050042710810</v>
-      </c>
-      <c r="N18" s="36" t="s">
-        <v>382</v>
-      </c>
+      <c r="M18" s="38"/>
+      <c r="N18" s="36"/>
       <c r="O18" s="36"/>
       <c r="P18" s="36"/>
       <c r="Q18" s="36"/>
@@ -5708,22 +5733,22 @@
         <v>109</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D19" s="36">
         <v>30</v>
       </c>
       <c r="E19" s="36"/>
-      <c r="F19" s="36" t="s">
-        <v>394</v>
-      </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
+      <c r="F19" s="40" t="s">
+        <v>393</v>
+      </c>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="42"/>
       <c r="K19" s="36"/>
       <c r="L19" s="36"/>
       <c r="M19" s="36"/>
@@ -5733,7 +5758,38 @@
       <c r="Q19" s="36"/>
       <c r="R19" s="36"/>
     </row>
+    <row r="20" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>422</v>
+      </c>
+      <c r="D20" s="36">
+        <v>19</v>
+      </c>
+      <c r="E20" s="36"/>
+      <c r="F20" s="40" t="s">
+        <v>426</v>
+      </c>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="F20:J20"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5870,17 +5926,17 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="43" t="s">
         <v>362</v>
       </c>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
     </row>
     <row r="5" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
@@ -6314,17 +6370,17 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="43" t="s">
         <v>362</v>
       </c>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="40"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -6687,17 +6743,17 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="43" t="s">
         <v>362</v>
       </c>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="40"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
     </row>
     <row r="4" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -7164,17 +7220,17 @@
       <c r="P3" s="16"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="43" t="s">
         <v>362</v>
       </c>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
@@ -7890,17 +7946,17 @@
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="43" t="s">
         <v>362</v>
       </c>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
     </row>
     <row r="5" spans="1:38" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
@@ -8690,17 +8746,17 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="43" t="s">
         <v>362</v>
       </c>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="40"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
     </row>
     <row r="4" spans="1:25" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">

</xml_diff>

<commit_message>
Update de documentação VCOM
</commit_message>
<xml_diff>
--- a/Documentos/Mapeamento das Fontes de Dados/2CX/MAPEAMENTO_2CX.xlsx
+++ b/Documentos/Mapeamento das Fontes de Dados/2CX/MAPEAMENTO_2CX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\int.matheus\Desktop\DW\Data-Warehouse\Documentos\Mapeamento das Fontes de Dados\2CX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C7B550-8E1A-466C-90E4-7E5C262C026C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CDC884-D2E5-4A53-A44F-AD9D07D8AF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="685" firstSheet="2" activeTab="3" xr2:uid="{40AA39DE-57CF-4226-99BA-0B59FFBB7B19}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="685" firstSheet="2" activeTab="2" xr2:uid="{40AA39DE-57CF-4226-99BA-0B59FFBB7B19}"/>
   </bookViews>
   <sheets>
     <sheet name="PAINEL" sheetId="18" state="hidden" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="454">
   <si>
     <t>CPF</t>
   </si>
@@ -1440,6 +1440,15 @@
 ORDER BY data_registro DESC
 LIMIT 10;</t>
   </si>
+  <si>
+    <t>EVENTO_ID</t>
+  </si>
+  <si>
+    <t>ID DO ACIONAMENTO NO DW</t>
+  </si>
+  <si>
+    <t>IDENTITY</t>
+  </si>
 </sst>
 </file>
 
@@ -1449,7 +1458,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1525,16 +1534,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="18">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1615,18 +1616,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1F4E78"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF44546A"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1638,7 +1627,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1688,21 +1677,6 @@
       </top>
       <bottom style="medium">
         <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1830,7 +1804,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1925,37 +1899,34 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1964,10 +1935,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2576,17 +2544,17 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="45" t="s">
         <v>362</v>
       </c>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
     </row>
     <row r="4" spans="1:25" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -3211,17 +3179,17 @@
       <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="45" t="s">
         <v>362</v>
       </c>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
     </row>
     <row r="5" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
@@ -3651,17 +3619,17 @@
       <c r="O3" s="16"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="J4" s="47" t="s">
+      <c r="J4" s="45" t="s">
         <v>362</v>
       </c>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
@@ -5885,10 +5853,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62AE222-1740-4697-9DDD-8C113A0027CC}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="70.77734375" defaultRowHeight="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5912,749 +5880,777 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="35" t="s">
         <v>311</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="35" t="s">
         <v>325</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="32" t="s">
         <v>326</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="32" t="s">
         <v>327</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="32" t="s">
         <v>328</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="32" t="s">
         <v>329</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="32" t="s">
         <v>330</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="32" t="s">
         <v>331</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="33" t="s">
         <v>332</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="33" t="s">
         <v>333</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="34" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>452</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2" s="34">
+        <v>19</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>426</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>453</v>
+      </c>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+    </row>
+    <row r="3" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B3" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C3" s="34" t="s">
         <v>310</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D3" s="34">
         <v>10</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36" t="s">
+      <c r="E3" s="34"/>
+      <c r="F3" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G3" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H3" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I3" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J3" s="34" t="s">
         <v>413</v>
       </c>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-    </row>
-    <row r="3" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+    </row>
+    <row r="4" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B4" s="34" t="s">
         <v>416</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C4" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D4" s="34">
         <v>20</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36" t="s">
+      <c r="E4" s="34"/>
+      <c r="F4" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G4" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H4" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I4" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J4" s="34" t="s">
         <v>396</v>
       </c>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-    </row>
-    <row r="4" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="36" t="s">
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+    </row>
+    <row r="5" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B5" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C5" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D5" s="34">
         <v>20</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G5" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H5" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I5" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J5" s="34" t="s">
         <v>396</v>
       </c>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-    </row>
-    <row r="5" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="36" t="s">
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+    </row>
+    <row r="6" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="34" t="s">
         <v>383</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B6" s="34" t="s">
         <v>417</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C6" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D6" s="34">
         <v>30</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G6" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H6" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I6" s="34" t="s">
         <v>404</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J6" s="34" t="s">
         <v>405</v>
       </c>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36" t="s">
+      <c r="K6" s="34"/>
+      <c r="L6" s="34" t="s">
         <v>407</v>
       </c>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="36"/>
-    </row>
-    <row r="6" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="36" t="s">
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+    </row>
+    <row r="7" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="34" t="s">
         <v>384</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B7" s="34" t="s">
         <v>385</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C7" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D7" s="34">
         <v>100</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G7" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H7" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="I7" s="34" t="s">
         <v>397</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J7" s="34" t="s">
         <v>406</v>
       </c>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36"/>
-    </row>
-    <row r="7" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="36" t="s">
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
+    </row>
+    <row r="8" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B8" s="34" t="s">
         <v>418</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C8" s="34" t="s">
         <v>419</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D8" s="34">
         <v>19</v>
       </c>
-      <c r="E7" s="36" t="s">
-        <v>426</v>
-      </c>
-      <c r="F7" s="36" t="s">
+      <c r="E8" s="34"/>
+      <c r="F8" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G8" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H8" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="I8" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J7" s="36" t="s">
+      <c r="J8" s="34" t="s">
         <v>395</v>
       </c>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="36"/>
-    </row>
-    <row r="8" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
+    </row>
+    <row r="9" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="34" t="s">
         <v>386</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B9" s="34" t="s">
         <v>387</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C9" s="34" t="s">
         <v>419</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D9" s="34">
         <v>19</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36" t="s">
+      <c r="E9" s="34"/>
+      <c r="F9" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G9" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H9" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I9" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J8" s="36" t="s">
+      <c r="J9" s="34" t="s">
         <v>398</v>
       </c>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="36"/>
-    </row>
-    <row r="9" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+    </row>
+    <row r="10" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="34" t="s">
         <v>388</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B10" s="34" t="s">
         <v>420</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C10" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D10" s="34">
         <v>200</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36" t="s">
+      <c r="E10" s="34"/>
+      <c r="F10" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G10" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H10" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I10" s="34" t="s">
         <v>409</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="J10" s="34" t="s">
         <v>406</v>
       </c>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36" t="s">
+      <c r="K10" s="34"/>
+      <c r="L10" s="34" t="s">
         <v>410</v>
       </c>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="36"/>
-    </row>
-    <row r="10" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="36" t="s">
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+    </row>
+    <row r="11" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="34" t="s">
         <v>389</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B11" s="34" t="s">
         <v>390</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C11" s="34" t="s">
         <v>419</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D11" s="34">
         <v>19</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36" t="s">
+      <c r="E11" s="34"/>
+      <c r="F11" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G11" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="H11" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I10" s="36" t="s">
+      <c r="I11" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J10" s="36" t="s">
+      <c r="J11" s="34" t="s">
         <v>403</v>
       </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="36"/>
-    </row>
-    <row r="11" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="36" t="s">
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+    </row>
+    <row r="12" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="34" t="s">
         <v>391</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B12" s="34" t="s">
         <v>392</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C12" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D12" s="34">
         <v>200</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36" t="s">
+      <c r="E12" s="34"/>
+      <c r="F12" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G12" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H11" s="36" t="s">
+      <c r="H12" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I11" s="36" t="s">
+      <c r="I12" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J11" s="36" t="s">
+      <c r="J12" s="34" t="s">
         <v>399</v>
       </c>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="36"/>
-    </row>
-    <row r="12" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="36" t="s">
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+    </row>
+    <row r="13" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B13" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C13" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D13" s="34">
         <v>250</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36" t="s">
+      <c r="E13" s="34"/>
+      <c r="F13" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G13" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="H13" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I12" s="36" t="s">
+      <c r="I13" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J12" s="36" t="s">
+      <c r="J13" s="34" t="s">
         <v>408</v>
       </c>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
-    </row>
-    <row r="13" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="36" t="s">
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+    </row>
+    <row r="14" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B14" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C14" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D14" s="34">
         <v>50</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36" t="s">
+      <c r="E14" s="34"/>
+      <c r="F14" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G13" s="36" t="s">
+      <c r="G14" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H13" s="36" t="s">
+      <c r="H14" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I13" s="36" t="s">
+      <c r="I14" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J13" s="36" t="s">
+      <c r="J14" s="34" t="s">
         <v>411</v>
       </c>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
-    </row>
-    <row r="14" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="36" t="s">
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+    </row>
+    <row r="15" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B15" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C15" s="34" t="s">
         <v>421</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D15" s="34">
         <v>19</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36" t="s">
+      <c r="E15" s="34"/>
+      <c r="F15" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G15" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H14" s="36" t="s">
+      <c r="H15" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I14" s="36" t="s">
+      <c r="I15" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J14" s="36" t="s">
+      <c r="J15" s="34" t="s">
         <v>400</v>
       </c>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="36"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="36"/>
-    </row>
-    <row r="15" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="36" t="s">
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+    </row>
+    <row r="16" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B16" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C16" s="34" t="s">
         <v>421</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D16" s="34">
         <v>19</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36" t="s">
+      <c r="E16" s="34"/>
+      <c r="F16" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G16" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H15" s="36" t="s">
+      <c r="H16" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I15" s="36" t="s">
+      <c r="I16" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J15" s="36" t="s">
+      <c r="J16" s="34" t="s">
         <v>401</v>
       </c>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
-    </row>
-    <row r="16" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="36" t="s">
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+    </row>
+    <row r="17" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B17" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C17" s="34" t="s">
         <v>421</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D17" s="34">
         <v>19</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36" t="s">
+      <c r="E17" s="34"/>
+      <c r="F17" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
-    </row>
-    <row r="17" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="36" t="s">
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+    </row>
+    <row r="18" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B18" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C18" s="34" t="s">
         <v>421</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D18" s="34">
         <v>19</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36" t="s">
+      <c r="E18" s="34"/>
+      <c r="F18" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
-    </row>
-    <row r="18" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="36" t="s">
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34"/>
+    </row>
+    <row r="19" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B19" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C19" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D19" s="34">
         <v>20</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36" t="s">
+      <c r="E19" s="34"/>
+      <c r="F19" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G19" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H18" s="36" t="s">
+      <c r="H19" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I18" s="36" t="s">
+      <c r="I19" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J18" s="36" t="s">
+      <c r="J19" s="34" t="s">
         <v>402</v>
       </c>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="36"/>
-    </row>
-    <row r="19" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="36" t="s">
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+    </row>
+    <row r="20" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B20" s="34" t="s">
         <v>415</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C20" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D19" s="36">
+      <c r="D20" s="34">
         <v>30</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="43" t="s">
+      <c r="E20" s="34"/>
+      <c r="F20" s="41" t="s">
         <v>393</v>
       </c>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="36"/>
-    </row>
-    <row r="20" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
+    </row>
+    <row r="21" spans="1:18" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C21" s="34" t="s">
         <v>421</v>
       </c>
-      <c r="D20" s="36">
+      <c r="D21" s="34">
         <v>19</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="43" t="s">
+      <c r="E21" s="34"/>
+      <c r="F21" s="41" t="s">
         <v>425</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F19:J19"/>
+  <mergeCells count="3">
     <mergeCell ref="F20:J20"/>
+    <mergeCell ref="F21:J21"/>
+    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6663,10 +6659,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11DB7E24-B45A-45EF-B179-ED76FBFF6766}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6692,536 +6688,563 @@
       <c r="A1" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="32" t="s">
         <v>311</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="35" t="s">
         <v>325</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="32" t="s">
         <v>326</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="32" t="s">
         <v>327</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="32" t="s">
         <v>328</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="32" t="s">
         <v>329</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="32" t="s">
         <v>330</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="32" t="s">
         <v>331</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="33" t="s">
         <v>332</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="33" t="s">
         <v>333</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>452</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2" s="34">
+        <v>19</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>426</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>453</v>
+      </c>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+    </row>
+    <row r="3" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B3" s="37" t="s">
         <v>427</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C3" s="34" t="s">
         <v>310</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D3" s="34">
         <v>10</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36" t="s">
+      <c r="E3" s="34"/>
+      <c r="F3" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G3" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H3" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I3" s="34" t="s">
         <v>428</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J3" s="34" t="s">
         <v>413</v>
       </c>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="46" t="s">
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="44" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
+    <row r="4" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B4" s="34" t="s">
         <v>416</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C4" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D4" s="34">
         <v>20</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36" t="s">
+      <c r="E4" s="34"/>
+      <c r="F4" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G4" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H4" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I4" s="34" t="s">
         <v>428</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J4" s="34" t="s">
         <v>429</v>
       </c>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="46"/>
-    </row>
-    <row r="4" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="36" t="s">
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="44"/>
+    </row>
+    <row r="5" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B5" s="34" t="s">
         <v>418</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C5" s="34" t="s">
         <v>419</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D5" s="34">
         <v>19</v>
       </c>
-      <c r="E4" s="36" t="s">
-        <v>426</v>
-      </c>
-      <c r="F4" s="36" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G5" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H5" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I5" s="34" t="s">
         <v>428</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J5" s="34" t="s">
         <v>395</v>
       </c>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="46"/>
-    </row>
-    <row r="5" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="36" t="s">
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="44"/>
+    </row>
+    <row r="6" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="34" t="s">
         <v>386</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B6" s="34" t="s">
         <v>387</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C6" s="34" t="s">
         <v>438</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D6" s="34">
         <v>8</v>
       </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G6" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H6" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I6" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J6" s="34" t="s">
         <v>398</v>
       </c>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="46"/>
-    </row>
-    <row r="6" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="36" t="s">
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="44"/>
+    </row>
+    <row r="7" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="34" t="s">
         <v>388</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B7" s="34" t="s">
         <v>420</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C7" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D7" s="34">
         <v>200</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G7" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H7" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="I7" s="34" t="s">
         <v>409</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J7" s="34" t="s">
         <v>406</v>
       </c>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36" t="s">
+      <c r="K7" s="34"/>
+      <c r="L7" s="34" t="s">
         <v>410</v>
       </c>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="46"/>
-    </row>
-    <row r="7" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="36" t="s">
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="44"/>
+    </row>
+    <row r="8" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B8" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C8" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D8" s="34">
         <v>20</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36" t="s">
+      <c r="E8" s="34"/>
+      <c r="F8" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G8" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H8" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="I8" s="34" t="s">
         <v>394</v>
       </c>
-      <c r="J7" s="36" t="s">
+      <c r="J8" s="34" t="s">
         <v>402</v>
       </c>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="46"/>
-    </row>
-    <row r="8" spans="1:15" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="44"/>
+    </row>
+    <row r="9" spans="1:15" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="34" t="s">
         <v>446</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>439</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C9" s="34" t="s">
         <v>419</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D9" s="34">
         <v>19</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36" t="s">
+      <c r="E9" s="34"/>
+      <c r="F9" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G9" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H9" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I9" s="34" t="s">
         <v>428</v>
       </c>
-      <c r="J8" s="36" t="s">
+      <c r="J9" s="34" t="s">
         <v>440</v>
       </c>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="46"/>
-    </row>
-    <row r="9" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="44"/>
+    </row>
+    <row r="10" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="34" t="s">
         <v>431</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B10" s="40" t="s">
         <v>434</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C10" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D10" s="34">
         <v>50</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36" t="s">
+      <c r="E10" s="34"/>
+      <c r="F10" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G10" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H10" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I10" s="34" t="s">
         <v>428</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="J10" s="34" t="s">
         <v>441</v>
       </c>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="46"/>
-    </row>
-    <row r="10" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="36" t="s">
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="44"/>
+    </row>
+    <row r="11" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="34" t="s">
         <v>430</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B11" s="40" t="s">
         <v>435</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C11" s="34" t="s">
         <v>438</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D11" s="34">
         <v>8</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36" t="s">
+      <c r="E11" s="34"/>
+      <c r="F11" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G11" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="H11" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I10" s="36" t="s">
+      <c r="I11" s="34" t="s">
         <v>428</v>
       </c>
-      <c r="J10" s="36" t="s">
+      <c r="J11" s="34" t="s">
         <v>442</v>
       </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="46"/>
-    </row>
-    <row r="11" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="36" t="s">
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="44"/>
+    </row>
+    <row r="12" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="34" t="s">
         <v>432</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B12" s="40" t="s">
         <v>436</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C12" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D12" s="34">
         <v>50</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36" t="s">
+      <c r="E12" s="34"/>
+      <c r="F12" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G12" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H11" s="36" t="s">
+      <c r="H12" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I11" s="36" t="s">
+      <c r="I12" s="34" t="s">
         <v>428</v>
       </c>
-      <c r="J11" s="36" t="s">
+      <c r="J12" s="34" t="s">
         <v>443</v>
       </c>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="46"/>
-    </row>
-    <row r="12" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="36" t="s">
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="44"/>
+    </row>
+    <row r="13" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="34" t="s">
         <v>433</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B13" s="40" t="s">
         <v>437</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C13" s="34" t="s">
         <v>438</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D13" s="34">
         <v>8</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36" t="s">
+      <c r="E13" s="34"/>
+      <c r="F13" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G13" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="H13" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I12" s="36" t="s">
+      <c r="I13" s="34" t="s">
         <v>428</v>
       </c>
-      <c r="J12" s="36" t="s">
+      <c r="J13" s="34" t="s">
         <v>444</v>
       </c>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="46"/>
-    </row>
-    <row r="13" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="40" t="s">
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="44"/>
+    </row>
+    <row r="14" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="38" t="s">
         <v>447</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B14" s="39" t="s">
         <v>445</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C14" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D14" s="34">
         <v>20</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36" t="s">
+      <c r="E14" s="34"/>
+      <c r="F14" s="34" t="s">
         <v>393</v>
       </c>
-      <c r="G13" s="36" t="s">
+      <c r="G14" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="H13" s="36" t="s">
+      <c r="H14" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="I13" s="36" t="s">
+      <c r="I14" s="34" t="s">
         <v>428</v>
       </c>
-      <c r="J13" s="36" t="s">
+      <c r="J14" s="34" t="s">
         <v>449</v>
       </c>
-      <c r="K13" s="36" t="s">
+      <c r="K14" s="34" t="s">
         <v>448</v>
       </c>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="46"/>
-    </row>
-    <row r="14" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="36" t="s">
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="44"/>
+    </row>
+    <row r="15" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B15" s="37" t="s">
         <v>415</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C15" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D15" s="34">
         <v>30</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="43" t="s">
+      <c r="E15" s="34"/>
+      <c r="F15" s="41" t="s">
         <v>393</v>
       </c>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="46"/>
-    </row>
-    <row r="15" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="40" t="s">
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="44"/>
+    </row>
+    <row r="16" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="38" t="s">
         <v>423</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B16" s="39" t="s">
         <v>424</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C16" s="34" t="s">
         <v>421</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D16" s="34">
         <v>19</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="43" t="s">
+      <c r="E16" s="34"/>
+      <c r="F16" s="41" t="s">
         <v>425</v>
       </c>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="46"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F14:J14"/>
+  <mergeCells count="4">
     <mergeCell ref="F15:J15"/>
-    <mergeCell ref="O2:O15"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="O3:O16"/>
+    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -7358,17 +7381,17 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="45" t="s">
         <v>362</v>
       </c>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
     </row>
     <row r="5" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
@@ -7802,17 +7825,17 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="45" t="s">
         <v>362</v>
       </c>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -8175,17 +8198,17 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="45" t="s">
         <v>362</v>
       </c>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
     </row>
     <row r="4" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -8652,17 +8675,17 @@
       <c r="P3" s="16"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="45" t="s">
         <v>362</v>
       </c>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
@@ -9378,17 +9401,17 @@
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="45" t="s">
         <v>362</v>
       </c>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
     </row>
     <row r="5" spans="1:38" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">

</xml_diff>